<commit_message>
Cost updates. Added Snakemake
</commit_message>
<xml_diff>
--- a/dataSources/P2G_FC_Costs.xlsx
+++ b/dataSources/P2G_FC_Costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\trevorb\repositories\Canada-U.S.-ElecTrade\dataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8869368-05B1-42FB-9BD5-ECE501E75F89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22239813-7C76-4F2C-99AA-EC2688560E06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40980" yWindow="3465" windowWidth="11280" windowHeight="5055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2G" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>CAPEX</t>
   </si>
@@ -47,6 +47,57 @@
   </si>
   <si>
     <t>Fuel</t>
+  </si>
+  <si>
+    <t>6809</t>
+  </si>
+  <si>
+    <t>6614</t>
+  </si>
+  <si>
+    <t>6420</t>
+  </si>
+  <si>
+    <t>6225</t>
+  </si>
+  <si>
+    <t>6031</t>
+  </si>
+  <si>
+    <t>5836</t>
+  </si>
+  <si>
+    <t>5642</t>
+  </si>
+  <si>
+    <t>5447</t>
+  </si>
+  <si>
+    <t>5253</t>
+  </si>
+  <si>
+    <t>5058</t>
+  </si>
+  <si>
+    <t>4864</t>
+  </si>
+  <si>
+    <t>4669</t>
+  </si>
+  <si>
+    <t>4475</t>
+  </si>
+  <si>
+    <t>4280</t>
+  </si>
+  <si>
+    <t>4086</t>
+  </si>
+  <si>
+    <t>3891</t>
+  </si>
+  <si>
+    <t>3696</t>
   </si>
 </sst>
 </file>
@@ -366,7 +417,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -396,8 +449,8 @@
       <c r="B2">
         <v>1500000000</v>
       </c>
-      <c r="C2">
-        <v>3700</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
       <c r="D2">
         <v>513889</v>
@@ -414,8 +467,8 @@
       <c r="B3">
         <v>1500000000</v>
       </c>
-      <c r="C3">
-        <v>3700</v>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
       <c r="D3">
         <v>513889</v>
@@ -432,8 +485,8 @@
       <c r="B4">
         <v>1426666667</v>
       </c>
-      <c r="C4">
-        <v>3700</v>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
       <c r="D4">
         <v>513889</v>
@@ -450,8 +503,8 @@
       <c r="B5">
         <v>1353333333</v>
       </c>
-      <c r="C5">
-        <v>3700</v>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
       <c r="D5">
         <v>513889</v>
@@ -468,8 +521,8 @@
       <c r="B6">
         <v>1280000000</v>
       </c>
-      <c r="C6">
-        <v>3700</v>
+      <c r="C6" t="s">
+        <v>8</v>
       </c>
       <c r="D6">
         <v>513889</v>
@@ -486,8 +539,8 @@
       <c r="B7">
         <v>1206666667</v>
       </c>
-      <c r="C7">
-        <v>3700</v>
+      <c r="C7" t="s">
+        <v>9</v>
       </c>
       <c r="D7">
         <v>513889</v>
@@ -504,8 +557,8 @@
       <c r="B8">
         <v>1133333333</v>
       </c>
-      <c r="C8">
-        <v>3700</v>
+      <c r="C8" t="s">
+        <v>10</v>
       </c>
       <c r="D8">
         <v>513889</v>
@@ -522,8 +575,8 @@
       <c r="B9">
         <v>1060000000</v>
       </c>
-      <c r="C9">
-        <v>3700</v>
+      <c r="C9" t="s">
+        <v>11</v>
       </c>
       <c r="D9">
         <v>513889</v>
@@ -540,8 +593,8 @@
       <c r="B10">
         <v>986666666.70000005</v>
       </c>
-      <c r="C10">
-        <v>3700</v>
+      <c r="C10" t="s">
+        <v>12</v>
       </c>
       <c r="D10">
         <v>513889</v>
@@ -558,8 +611,8 @@
       <c r="B11">
         <v>913333333.29999995</v>
       </c>
-      <c r="C11">
-        <v>3700</v>
+      <c r="C11" t="s">
+        <v>13</v>
       </c>
       <c r="D11">
         <v>513889</v>
@@ -576,8 +629,8 @@
       <c r="B12">
         <v>840000000</v>
       </c>
-      <c r="C12">
-        <v>3700</v>
+      <c r="C12" t="s">
+        <v>14</v>
       </c>
       <c r="D12">
         <v>513889</v>
@@ -594,8 +647,8 @@
       <c r="B13">
         <v>766666666.70000005</v>
       </c>
-      <c r="C13">
-        <v>3700</v>
+      <c r="C13" t="s">
+        <v>15</v>
       </c>
       <c r="D13">
         <v>513889</v>
@@ -612,8 +665,8 @@
       <c r="B14">
         <v>693333333.29999995</v>
       </c>
-      <c r="C14">
-        <v>3700</v>
+      <c r="C14" t="s">
+        <v>16</v>
       </c>
       <c r="D14">
         <v>513889</v>
@@ -630,8 +683,8 @@
       <c r="B15">
         <v>620000000</v>
       </c>
-      <c r="C15">
-        <v>3700</v>
+      <c r="C15" t="s">
+        <v>17</v>
       </c>
       <c r="D15">
         <v>513889</v>
@@ -648,8 +701,8 @@
       <c r="B16">
         <v>546666666.70000005</v>
       </c>
-      <c r="C16">
-        <v>3700</v>
+      <c r="C16" t="s">
+        <v>18</v>
       </c>
       <c r="D16">
         <v>513889</v>
@@ -666,8 +719,8 @@
       <c r="B17">
         <v>473333333.30000001</v>
       </c>
-      <c r="C17">
-        <v>3700</v>
+      <c r="C17" t="s">
+        <v>19</v>
       </c>
       <c r="D17">
         <v>513889</v>
@@ -684,8 +737,8 @@
       <c r="B18">
         <v>400000000</v>
       </c>
-      <c r="C18">
-        <v>3700</v>
+      <c r="C18" t="s">
+        <v>20</v>
       </c>
       <c r="D18">
         <v>513889</v>
@@ -702,8 +755,8 @@
       <c r="B19">
         <v>400000000</v>
       </c>
-      <c r="C19">
-        <v>3700</v>
+      <c r="C19" t="s">
+        <v>20</v>
       </c>
       <c r="D19">
         <v>513889</v>
@@ -720,8 +773,8 @@
       <c r="B20">
         <v>400000000</v>
       </c>
-      <c r="C20">
-        <v>3700</v>
+      <c r="C20" t="s">
+        <v>20</v>
       </c>
       <c r="D20">
         <v>513889</v>
@@ -738,8 +791,8 @@
       <c r="B21">
         <v>400000000</v>
       </c>
-      <c r="C21">
-        <v>3700</v>
+      <c r="C21" t="s">
+        <v>20</v>
       </c>
       <c r="D21">
         <v>513889</v>
@@ -756,8 +809,8 @@
       <c r="B22">
         <v>400000000</v>
       </c>
-      <c r="C22">
-        <v>3700</v>
+      <c r="C22" t="s">
+        <v>20</v>
       </c>
       <c r="D22">
         <v>513889</v>
@@ -774,8 +827,8 @@
       <c r="B23">
         <v>400000000</v>
       </c>
-      <c r="C23">
-        <v>3700</v>
+      <c r="C23" t="s">
+        <v>20</v>
       </c>
       <c r="D23">
         <v>513889</v>
@@ -792,8 +845,8 @@
       <c r="B24">
         <v>400000000</v>
       </c>
-      <c r="C24">
-        <v>3700</v>
+      <c r="C24" t="s">
+        <v>20</v>
       </c>
       <c r="D24">
         <v>513889</v>
@@ -810,8 +863,8 @@
       <c r="B25">
         <v>400000000</v>
       </c>
-      <c r="C25">
-        <v>3700</v>
+      <c r="C25" t="s">
+        <v>20</v>
       </c>
       <c r="D25">
         <v>513889</v>
@@ -828,8 +881,8 @@
       <c r="B26">
         <v>400000000</v>
       </c>
-      <c r="C26">
-        <v>3700</v>
+      <c r="C26" t="s">
+        <v>20</v>
       </c>
       <c r="D26">
         <v>513889</v>
@@ -846,8 +899,8 @@
       <c r="B27">
         <v>400000000</v>
       </c>
-      <c r="C27">
-        <v>3700</v>
+      <c r="C27" t="s">
+        <v>20</v>
       </c>
       <c r="D27">
         <v>513889</v>
@@ -864,8 +917,8 @@
       <c r="B28">
         <v>400000000</v>
       </c>
-      <c r="C28">
-        <v>3700</v>
+      <c r="C28" t="s">
+        <v>20</v>
       </c>
       <c r="D28">
         <v>513889</v>
@@ -882,8 +935,8 @@
       <c r="B29">
         <v>400000000</v>
       </c>
-      <c r="C29">
-        <v>3700</v>
+      <c r="C29" t="s">
+        <v>20</v>
       </c>
       <c r="D29">
         <v>513889</v>
@@ -900,8 +953,8 @@
       <c r="B30">
         <v>400000000</v>
       </c>
-      <c r="C30">
-        <v>3700</v>
+      <c r="C30" t="s">
+        <v>20</v>
       </c>
       <c r="D30">
         <v>513889</v>
@@ -918,8 +971,8 @@
       <c r="B31">
         <v>400000000</v>
       </c>
-      <c r="C31">
-        <v>3700</v>
+      <c r="C31" t="s">
+        <v>20</v>
       </c>
       <c r="D31">
         <v>513889</v>
@@ -936,8 +989,8 @@
       <c r="B32">
         <v>400000000</v>
       </c>
-      <c r="C32">
-        <v>3700</v>
+      <c r="C32" t="s">
+        <v>20</v>
       </c>
       <c r="D32">
         <v>513889</v>
@@ -954,8 +1007,8 @@
       <c r="B33">
         <v>400000000</v>
       </c>
-      <c r="C33">
-        <v>3700</v>
+      <c r="C33" t="s">
+        <v>20</v>
       </c>
       <c r="D33">
         <v>513889</v>

</xml_diff>

<commit_message>
Updated cost and emission units
</commit_message>
<xml_diff>
--- a/dataSources/P2G_FC_Costs.xlsx
+++ b/dataSources/P2G_FC_Costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\trevorb\repositories\Canada-U.S.-ElecTrade\dataSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22239813-7C76-4F2C-99AA-EC2688560E06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE5E440-D120-4B10-82A5-CCFFDEAE9526}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2G" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>CAPEX</t>
   </si>
@@ -48,62 +48,14 @@
   <si>
     <t>Fuel</t>
   </si>
-  <si>
-    <t>6809</t>
-  </si>
-  <si>
-    <t>6614</t>
-  </si>
-  <si>
-    <t>6420</t>
-  </si>
-  <si>
-    <t>6225</t>
-  </si>
-  <si>
-    <t>6031</t>
-  </si>
-  <si>
-    <t>5836</t>
-  </si>
-  <si>
-    <t>5642</t>
-  </si>
-  <si>
-    <t>5447</t>
-  </si>
-  <si>
-    <t>5253</t>
-  </si>
-  <si>
-    <t>5058</t>
-  </si>
-  <si>
-    <t>4864</t>
-  </si>
-  <si>
-    <t>4669</t>
-  </si>
-  <si>
-    <t>4475</t>
-  </si>
-  <si>
-    <t>4280</t>
-  </si>
-  <si>
-    <t>4086</t>
-  </si>
-  <si>
-    <t>3891</t>
-  </si>
-  <si>
-    <t>3696</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,7 +371,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -446,14 +399,14 @@
       <c r="A2">
         <v>2019</v>
       </c>
-      <c r="B2">
-        <v>1500000000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="B2" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C2">
+        <v>6.8089999999999999E-3</v>
       </c>
       <c r="D2">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -464,14 +417,14 @@
         <f>A2+1</f>
         <v>2020</v>
       </c>
-      <c r="B3">
-        <v>1500000000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="B3" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C3">
+        <v>6.6140000000000001E-3</v>
       </c>
       <c r="D3">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -482,14 +435,14 @@
         <f t="shared" ref="A4:A33" si="0">A3+1</f>
         <v>2021</v>
       </c>
-      <c r="B4">
-        <v>1426666667</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
+      <c r="B4" s="1">
+        <v>1426.666667</v>
+      </c>
+      <c r="C4">
+        <v>6.4200000000000004E-3</v>
       </c>
       <c r="D4">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -500,14 +453,14 @@
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="B5">
-        <v>1353333333</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+      <c r="B5" s="1">
+        <v>1353.333333</v>
+      </c>
+      <c r="C5">
+        <v>6.2249999999999996E-3</v>
       </c>
       <c r="D5">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -518,14 +471,14 @@
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="B6">
-        <v>1280000000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
+      <c r="B6" s="1">
+        <v>1280</v>
+      </c>
+      <c r="C6">
+        <v>6.0309999999999999E-3</v>
       </c>
       <c r="D6">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -536,14 +489,14 @@
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="B7">
-        <v>1206666667</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
+      <c r="B7" s="1">
+        <v>1206.666667</v>
+      </c>
+      <c r="C7">
+        <v>5.836E-3</v>
       </c>
       <c r="D7">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -554,14 +507,14 @@
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
-      <c r="B8">
-        <v>1133333333</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
+      <c r="B8" s="1">
+        <v>1133.333333</v>
+      </c>
+      <c r="C8">
+        <v>5.6420000000000003E-3</v>
       </c>
       <c r="D8">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -572,14 +525,14 @@
         <f t="shared" si="0"/>
         <v>2026</v>
       </c>
-      <c r="B9">
-        <v>1060000000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
+      <c r="B9" s="1">
+        <v>1060</v>
+      </c>
+      <c r="C9">
+        <v>5.4469999999999996E-3</v>
       </c>
       <c r="D9">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -590,14 +543,14 @@
         <f t="shared" si="0"/>
         <v>2027</v>
       </c>
-      <c r="B10">
-        <v>986666666.70000005</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
+      <c r="B10" s="1">
+        <v>986.66666670000006</v>
+      </c>
+      <c r="C10">
+        <v>5.2529999999999999E-3</v>
       </c>
       <c r="D10">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -608,14 +561,14 @@
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="B11">
-        <v>913333333.29999995</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
+      <c r="B11" s="1">
+        <v>913.33333329999994</v>
+      </c>
+      <c r="C11">
+        <v>5.058E-3</v>
       </c>
       <c r="D11">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -626,14 +579,14 @@
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="B12">
-        <v>840000000</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
+      <c r="B12" s="1">
+        <v>840</v>
+      </c>
+      <c r="C12">
+        <v>4.8640000000000003E-3</v>
       </c>
       <c r="D12">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -644,14 +597,14 @@
         <f t="shared" si="0"/>
         <v>2030</v>
       </c>
-      <c r="B13">
-        <v>766666666.70000005</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
+      <c r="B13" s="1">
+        <v>766.66666670000006</v>
+      </c>
+      <c r="C13">
+        <v>4.6690000000000004E-3</v>
       </c>
       <c r="D13">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -662,14 +615,14 @@
         <f t="shared" si="0"/>
         <v>2031</v>
       </c>
-      <c r="B14">
-        <v>693333333.29999995</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
+      <c r="B14" s="1">
+        <v>693.33333329999994</v>
+      </c>
+      <c r="C14">
+        <v>4.4749999999999998E-3</v>
       </c>
       <c r="D14">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -680,14 +633,14 @@
         <f t="shared" si="0"/>
         <v>2032</v>
       </c>
-      <c r="B15">
-        <v>620000000</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
+      <c r="B15" s="1">
+        <v>620</v>
+      </c>
+      <c r="C15">
+        <v>4.28E-3</v>
       </c>
       <c r="D15">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -698,14 +651,14 @@
         <f t="shared" si="0"/>
         <v>2033</v>
       </c>
-      <c r="B16">
-        <v>546666666.70000005</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
+      <c r="B16" s="1">
+        <v>546.66666670000006</v>
+      </c>
+      <c r="C16">
+        <v>4.0860000000000002E-3</v>
       </c>
       <c r="D16">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -716,14 +669,14 @@
         <f t="shared" si="0"/>
         <v>2034</v>
       </c>
-      <c r="B17">
-        <v>473333333.30000001</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
+      <c r="B17" s="1">
+        <v>473.33333329999999</v>
+      </c>
+      <c r="C17">
+        <v>3.8909999999999999E-3</v>
       </c>
       <c r="D17">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -734,14 +687,14 @@
         <f t="shared" si="0"/>
         <v>2035</v>
       </c>
-      <c r="B18">
-        <v>400000000</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
+      <c r="B18" s="1">
+        <v>400</v>
+      </c>
+      <c r="C18">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D18">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -752,14 +705,14 @@
         <f t="shared" si="0"/>
         <v>2036</v>
       </c>
-      <c r="B19">
-        <v>400000000</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
+      <c r="B19" s="1">
+        <v>400</v>
+      </c>
+      <c r="C19">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D19">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -770,14 +723,14 @@
         <f t="shared" si="0"/>
         <v>2037</v>
       </c>
-      <c r="B20">
-        <v>400000000</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
+      <c r="B20" s="1">
+        <v>400</v>
+      </c>
+      <c r="C20">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D20">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -788,14 +741,14 @@
         <f t="shared" si="0"/>
         <v>2038</v>
       </c>
-      <c r="B21">
-        <v>400000000</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
+      <c r="B21" s="1">
+        <v>400</v>
+      </c>
+      <c r="C21">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D21">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -806,14 +759,14 @@
         <f t="shared" si="0"/>
         <v>2039</v>
       </c>
-      <c r="B22">
-        <v>400000000</v>
-      </c>
-      <c r="C22" t="s">
-        <v>20</v>
+      <c r="B22" s="1">
+        <v>400</v>
+      </c>
+      <c r="C22">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D22">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -824,14 +777,14 @@
         <f t="shared" si="0"/>
         <v>2040</v>
       </c>
-      <c r="B23">
-        <v>400000000</v>
-      </c>
-      <c r="C23" t="s">
-        <v>20</v>
+      <c r="B23" s="1">
+        <v>400</v>
+      </c>
+      <c r="C23">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D23">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -842,14 +795,14 @@
         <f t="shared" si="0"/>
         <v>2041</v>
       </c>
-      <c r="B24">
-        <v>400000000</v>
-      </c>
-      <c r="C24" t="s">
-        <v>20</v>
+      <c r="B24" s="1">
+        <v>400</v>
+      </c>
+      <c r="C24">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D24">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -860,14 +813,14 @@
         <f t="shared" si="0"/>
         <v>2042</v>
       </c>
-      <c r="B25">
-        <v>400000000</v>
-      </c>
-      <c r="C25" t="s">
-        <v>20</v>
+      <c r="B25" s="1">
+        <v>400</v>
+      </c>
+      <c r="C25">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D25">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -878,14 +831,14 @@
         <f t="shared" si="0"/>
         <v>2043</v>
       </c>
-      <c r="B26">
-        <v>400000000</v>
-      </c>
-      <c r="C26" t="s">
-        <v>20</v>
+      <c r="B26" s="1">
+        <v>400</v>
+      </c>
+      <c r="C26">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D26">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -896,14 +849,14 @@
         <f t="shared" si="0"/>
         <v>2044</v>
       </c>
-      <c r="B27">
-        <v>400000000</v>
-      </c>
-      <c r="C27" t="s">
-        <v>20</v>
+      <c r="B27" s="1">
+        <v>400</v>
+      </c>
+      <c r="C27">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D27">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -914,14 +867,14 @@
         <f t="shared" si="0"/>
         <v>2045</v>
       </c>
-      <c r="B28">
-        <v>400000000</v>
-      </c>
-      <c r="C28" t="s">
-        <v>20</v>
+      <c r="B28" s="1">
+        <v>400</v>
+      </c>
+      <c r="C28">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D28">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -932,14 +885,14 @@
         <f t="shared" si="0"/>
         <v>2046</v>
       </c>
-      <c r="B29">
-        <v>400000000</v>
-      </c>
-      <c r="C29" t="s">
-        <v>20</v>
+      <c r="B29" s="1">
+        <v>400</v>
+      </c>
+      <c r="C29">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D29">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -950,14 +903,14 @@
         <f t="shared" si="0"/>
         <v>2047</v>
       </c>
-      <c r="B30">
-        <v>400000000</v>
-      </c>
-      <c r="C30" t="s">
-        <v>20</v>
+      <c r="B30" s="1">
+        <v>400</v>
+      </c>
+      <c r="C30">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D30">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -968,14 +921,14 @@
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
-      <c r="B31">
-        <v>400000000</v>
-      </c>
-      <c r="C31" t="s">
-        <v>20</v>
+      <c r="B31" s="1">
+        <v>400</v>
+      </c>
+      <c r="C31">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D31">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -986,14 +939,14 @@
         <f>A31+1</f>
         <v>2049</v>
       </c>
-      <c r="B32">
-        <v>400000000</v>
-      </c>
-      <c r="C32" t="s">
-        <v>20</v>
+      <c r="B32" s="1">
+        <v>400</v>
+      </c>
+      <c r="C32">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D32">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1004,14 +957,14 @@
         <f t="shared" si="0"/>
         <v>2050</v>
       </c>
-      <c r="B33">
-        <v>400000000</v>
-      </c>
-      <c r="C33" t="s">
-        <v>20</v>
+      <c r="B33" s="1">
+        <v>400</v>
+      </c>
+      <c r="C33">
+        <v>3.6960000000000001E-3</v>
       </c>
       <c r="D33">
-        <v>513889</v>
+        <v>0.51388900000000004</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1027,7 +980,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1057,10 +1010,10 @@
         <v>2019</v>
       </c>
       <c r="B2">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C2">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1075,10 +1028,10 @@
         <v>2020</v>
       </c>
       <c r="B3">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C3">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1093,10 +1046,10 @@
         <v>2021</v>
       </c>
       <c r="B4">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C4">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1111,10 +1064,10 @@
         <v>2022</v>
       </c>
       <c r="B5">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C5">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1129,10 +1082,10 @@
         <v>2023</v>
       </c>
       <c r="B6">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C6">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1147,10 +1100,10 @@
         <v>2024</v>
       </c>
       <c r="B7">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C7">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1165,10 +1118,10 @@
         <v>2025</v>
       </c>
       <c r="B8">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C8">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1183,10 +1136,10 @@
         <v>2026</v>
       </c>
       <c r="B9">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C9">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1201,10 +1154,10 @@
         <v>2027</v>
       </c>
       <c r="B10">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C10">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1219,10 +1172,10 @@
         <v>2028</v>
       </c>
       <c r="B11">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C11">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1237,10 +1190,10 @@
         <v>2029</v>
       </c>
       <c r="B12">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C12">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1255,10 +1208,10 @@
         <v>2030</v>
       </c>
       <c r="B13">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C13">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1273,10 +1226,10 @@
         <v>2031</v>
       </c>
       <c r="B14">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C14">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1291,10 +1244,10 @@
         <v>2032</v>
       </c>
       <c r="B15">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C15">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1309,10 +1262,10 @@
         <v>2033</v>
       </c>
       <c r="B16">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C16">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1327,10 +1280,10 @@
         <v>2034</v>
       </c>
       <c r="B17">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C17">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1345,10 +1298,10 @@
         <v>2035</v>
       </c>
       <c r="B18">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C18">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1363,10 +1316,10 @@
         <v>2036</v>
       </c>
       <c r="B19">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C19">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1381,10 +1334,10 @@
         <v>2037</v>
       </c>
       <c r="B20">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C20">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1399,10 +1352,10 @@
         <v>2038</v>
       </c>
       <c r="B21">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C21">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1417,10 +1370,10 @@
         <v>2039</v>
       </c>
       <c r="B22">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C22">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1435,10 +1388,10 @@
         <v>2040</v>
       </c>
       <c r="B23">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C23">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1453,10 +1406,10 @@
         <v>2041</v>
       </c>
       <c r="B24">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C24">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1471,10 +1424,10 @@
         <v>2042</v>
       </c>
       <c r="B25">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C25">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1489,10 +1442,10 @@
         <v>2043</v>
       </c>
       <c r="B26">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C26">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1507,10 +1460,10 @@
         <v>2044</v>
       </c>
       <c r="B27">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C27">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1525,10 +1478,10 @@
         <v>2045</v>
       </c>
       <c r="B28">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C28">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1543,10 +1496,10 @@
         <v>2046</v>
       </c>
       <c r="B29">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C29">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1561,10 +1514,10 @@
         <v>2047</v>
       </c>
       <c r="B30">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C30">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1579,10 +1532,10 @@
         <v>2048</v>
       </c>
       <c r="B31">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C31">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1597,10 +1550,10 @@
         <v>2049</v>
       </c>
       <c r="B32">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C32">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1615,10 +1568,10 @@
         <v>2050</v>
       </c>
       <c r="B33">
-        <v>2400000000</v>
+        <v>2400</v>
       </c>
       <c r="C33">
-        <v>72000000</v>
+        <v>72</v>
       </c>
       <c r="D33">
         <v>0</v>

</xml_diff>